<commit_message>
updated excel for Fizzbuzz
</commit_message>
<xml_diff>
--- a/leettracker.xlsx
+++ b/leettracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/M_726661/Desktop/leetcode/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E81D3598-4947-8E48-8F6A-F5BFF7BA01B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B72024DA-D278-2A4A-9CCF-62985BD8B031}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{FD720952-DA5D-8A45-A7FA-5933E7B3BA3B}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="38">
   <si>
     <t>Problem Number</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Move Zeroes</t>
+  </si>
+  <si>
+    <t>12th Aug</t>
+  </si>
+  <si>
+    <t>FizzBuzz</t>
   </si>
 </sst>
 </file>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD2F190A-1005-B946-AB9B-42EEF2292475}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -811,6 +817,23 @@
         <v>16</v>
       </c>
     </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>412</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>